<commit_message>
Added Missing values, fixed silkscreen and OLED spacing
</commit_message>
<xml_diff>
--- a/Hardware/Basic/G4_TechWatch-BASIC-BOM.xlsx
+++ b/Hardware/Basic/G4_TechWatch-BASIC-BOM.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/Git/Tasks-Tutorials-Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notbe\Documents\Milestones_2022\G4_TechWatch\Hardware\Basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F0319-899B-F545-ABC0-B856698FB7B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76AA556-1B8B-42CB-A6E1-E86281B8612E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8358" yWindow="2196" windowWidth="11040" windowHeight="8064" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -258,40 +266,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{42ADFC76-2A16-3F4B-9937-20E1DF8DC9D9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{92578C3E-17AC-CF40-B33B-C67DBD723ACA}">
       <text>
         <r>
@@ -392,6 +366,435 @@
       </text>
     </comment>
     <comment ref="B8" authorId="0" shapeId="0" xr:uid="{7F187FCD-1E21-9644-AE5D-0FA5E52F65FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{BE95A23C-5D44-4141-91FF-84C4E1A72F65}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{3DB14386-B4E0-4261-A7E4-616F68F02C41}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{066B8278-E805-49D0-AD2C-C7FFCF94CE6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{6D5D37B5-2117-4B82-B72F-DC0EC8D73593}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{2745A1A9-C9F6-4026-BF37-CF11CB9A6090}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{A6989BAE-6D77-4148-8919-7BE3A98318FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{8FA952EA-1715-4C5C-A388-2B24092F2891}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{E28FA541-1B89-4BC2-AD97-235C18534E0E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{ECD91380-8AB4-4A7A-BE29-AB54508DD76D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{94E710EA-D39D-4DF5-ACFD-B03A80CB32AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{94D1E525-3E99-4E21-B074-2FB9AB9BB53A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{3F6C3C9D-DE28-4C4A-B953-A12B578D729B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Orlando Hoilett:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is just an example to show you what information to list and how to list them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{26FB429E-E746-47DC-AE06-EC47B5D5906A}">
       <text>
         <r>
           <rPr>
@@ -429,7 +832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>BOM #</t>
   </si>
@@ -470,9 +873,6 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -494,15 +894,6 @@
     <t>1uF capacitor</t>
   </si>
   <si>
-    <t>LM358</t>
-  </si>
-  <si>
-    <t>Photoresistor</t>
-  </si>
-  <si>
-    <t>9V Battery Connector</t>
-  </si>
-  <si>
     <t>1µF ±10% 25V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
   </si>
   <si>
@@ -515,87 +906,18 @@
     <t>Per 100</t>
   </si>
   <si>
-    <t>White  LED Indication - Discrete 2.9V Radial</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>Radial</t>
-  </si>
-  <si>
-    <t>American Bright Optoelectronics Corporation</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02-ND</t>
-  </si>
-  <si>
-    <t>White LED</t>
-  </si>
-  <si>
-    <t>Battery Connector, Snap 9V 1 Cell Wire Leads - 4" (101.6mm)</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>81-4</t>
-  </si>
-  <si>
-    <t>36-81-4-ND</t>
-  </si>
-  <si>
-    <t>9V</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>General Purpose Amplifier 2 Circuit  8-SOIC</t>
-  </si>
-  <si>
-    <t>8-SOIC</t>
-  </si>
-  <si>
-    <t>LM358DR</t>
-  </si>
-  <si>
-    <t>296-1014-1-ND</t>
-  </si>
-  <si>
-    <t>OP1</t>
-  </si>
-  <si>
     <t>Total (in Bulk)</t>
   </si>
   <si>
-    <t>CDS Cell 520nm 27 ~ 60kOhms @ 10 lux</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Advanced Photonix</t>
-  </si>
-  <si>
-    <t>PDV-P8104</t>
-  </si>
-  <si>
-    <t>PDV-P8104-ND</t>
-  </si>
-  <si>
     <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
   </si>
   <si>
-    <t>R1,R2,R3</t>
-  </si>
-  <si>
     <t>RMCF0603FT10K0</t>
   </si>
   <si>
@@ -603,6 +925,124 @@
   </si>
   <si>
     <t>Design Name -- Revision Code / Designer or Organization Name</t>
+  </si>
+  <si>
+    <t>NRF52832</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>BLE Capable Microcontroller</t>
+  </si>
+  <si>
+    <t>41-SMD Module</t>
+  </si>
+  <si>
+    <t>Raytac</t>
+  </si>
+  <si>
+    <t>MDBT42Q-512KV2</t>
+  </si>
+  <si>
+    <t>3271-MDBT42Q-512KV2-ND</t>
+  </si>
+  <si>
+    <t>100k resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>1k resistor</t>
+  </si>
+  <si>
+    <t>R4,R5</t>
+  </si>
+  <si>
+    <t>R3,R7,R8,R9</t>
+  </si>
+  <si>
+    <t>R1,R2,R10,R11</t>
+  </si>
+  <si>
+    <t>390k resistor</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>10uF capacitor</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>300pF capacitor</t>
+  </si>
+  <si>
+    <t>C5,C6</t>
+  </si>
+  <si>
+    <t>4.7uF capacitor</t>
+  </si>
+  <si>
+    <t>C7,C10</t>
+  </si>
+  <si>
+    <t>100nF capacitor</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C2,C12</t>
+  </si>
+  <si>
+    <t>C1,C8,C9,C18</t>
+  </si>
+  <si>
+    <t>BUTTON-GULLWING</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>SW3,SW4,SW5</t>
+  </si>
+  <si>
+    <t>TACTILE_SWITCH_SMD_6.2MM_TALL</t>
+  </si>
+  <si>
+    <t>10uH Inductor</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>XTAL1</t>
+  </si>
+  <si>
+    <t>32.768kHz Oscillator</t>
+  </si>
+  <si>
+    <t>2-SMD.NOLEAD.2.0MMTO1.2MM (Version 1 + Edits)</t>
+  </si>
+  <si>
+    <t>RED SMD LED</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>BLUE SMD LED</t>
   </si>
 </sst>
 </file>
@@ -684,11 +1124,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI Historic"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -856,7 +1295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,6 +1332,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1314,32 +1757,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.34765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.84765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.84765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1484375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="15.94921875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.84765625" style="1"/>
+    <col min="12" max="12" width="6.6484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.84765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="14.7" x14ac:dyDescent="0.65">
       <c r="A1" s="12" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1352,21 +1795,21 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="6">
         <f>SUM(M3:M77)</f>
-        <v>2.48</v>
+        <v>10.700000000000001</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="O1" s="6">
         <f>SUM(O3:O77)</f>
-        <v>1.1271</v>
+        <v>9.9516000000000009</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1398,312 +1841,740 @@
         <v>8</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K3" s="10">
-        <v>0.38</v>
+        <v>9.9</v>
       </c>
       <c r="L3" s="11">
         <v>1</v>
       </c>
       <c r="M3" s="10">
         <f t="shared" ref="M3:M8" si="0">K3*L3</f>
-        <v>0.38</v>
+        <v>9.9</v>
       </c>
       <c r="N3" s="10">
-        <v>0.1391</v>
+        <v>9.9</v>
       </c>
       <c r="O3" s="10">
         <f t="shared" ref="O3:O7" si="1">L3*N3</f>
-        <v>0.1391</v>
+        <v>9.9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>22</v>
+      <c r="B4" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>48</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>51</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.89</v>
-      </c>
-      <c r="L4" s="11">
-        <v>1</v>
-      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="10">
         <f t="shared" si="0"/>
-        <v>0.89</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0.46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N4" s="10"/>
       <c r="O4" s="10">
         <f t="shared" si="1"/>
-        <v>0.46</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L5" s="11">
-        <v>1</v>
-      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.3982</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N5" s="10"/>
       <c r="O5" s="10">
         <f t="shared" si="1"/>
-        <v>0.3982</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>32</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0.26</v>
-      </c>
-      <c r="L6" s="11">
-        <v>1</v>
-      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="10">
         <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-      <c r="N6" s="10">
-        <v>9.0899999999999995E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N6" s="10"/>
       <c r="O6" s="10">
         <f t="shared" si="1"/>
-        <v>9.0899999999999995E-2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="K7" s="10">
         <v>0.1</v>
       </c>
       <c r="L7" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="N7" s="10">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O7" s="10">
         <f t="shared" si="1"/>
-        <v>2.0399999999999998E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="H8" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K8" s="10">
         <v>0.1</v>
       </c>
-      <c r="L8" s="11">
-        <v>1</v>
-      </c>
+      <c r="L8" s="11"/>
       <c r="M8" s="10">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="10">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="O8" s="10">
         <f>L8*N8</f>
-        <v>1.8499999999999999E-2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="11">
+        <v>4</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" ref="M9:M10" si="2">K9*L9</f>
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="10">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="O9" s="10">
+        <f>L9*N9</f>
+        <v>2.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
+        <f t="shared" ref="O10" si="3">L10*N10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="10">
+        <f t="shared" ref="M11:M15" si="4">K11*L11</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
+        <f t="shared" ref="O11" si="5">L11*N11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10">
+        <f>L12*N12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="M13" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10">
+        <f>L13*N13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="M14" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10">
+        <f>L14*N14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="M15" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10">
+        <f>L15*N15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="M16" s="10">
+        <f t="shared" ref="M16:M17" si="6">K16*L16</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10">
+        <f>L16*N16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="M17" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10">
+        <f>L17*N17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="M18" s="10">
+        <f t="shared" ref="M18:M22" si="7">K18*L18</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10">
+        <f>L18*N18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="M19" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10">
+        <f t="shared" ref="O19:O22" si="8">L19*N19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="M20" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="M21" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A22" s="8">
+        <v>20</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="M22" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1711,8 +2582,8 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
BOM Ver 1 Finished
</commit_message>
<xml_diff>
--- a/Hardware/Basic/G4_TechWatch-BASIC-BOM.xlsx
+++ b/Hardware/Basic/G4_TechWatch-BASIC-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notbe\Documents\Milestones_2022\G4_TechWatch\Hardware\Basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76AA556-1B8B-42CB-A6E1-E86281B8612E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C10691-0E4C-443B-A2C4-9EEB3279E2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8358" yWindow="2196" windowWidth="11040" windowHeight="8064" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{066B8278-E805-49D0-AD2C-C7FFCF94CE6F}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{6D5D37B5-2117-4B82-B72F-DC0EC8D73593}">
       <text>
         <r>
           <rPr>
@@ -497,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{6D5D37B5-2117-4B82-B72F-DC0EC8D73593}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{2745A1A9-C9F6-4026-BF37-CF11CB9A6090}">
       <text>
         <r>
           <rPr>
@@ -530,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{2745A1A9-C9F6-4026-BF37-CF11CB9A6090}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{A6989BAE-6D77-4148-8919-7BE3A98318FB}">
       <text>
         <r>
           <rPr>
@@ -563,40 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{A6989BAE-6D77-4148-8919-7BE3A98318FB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{8FA952EA-1715-4C5C-A388-2B24092F2891}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{8FA952EA-1715-4C5C-A388-2B24092F2891}">
       <text>
         <r>
           <rPr>
@@ -832,7 +799,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
   <si>
     <t>BOM #</t>
   </si>
@@ -909,9 +876,6 @@
     <t>LED1</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>Total (in Bulk)</t>
   </si>
   <si>
@@ -957,10 +921,6 @@
     <t>RMCF0603FT100K</t>
   </si>
   <si>
-    <t xml:space="preserve">
-100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-  </si>
-  <si>
     <t>1k resistor</t>
   </si>
   <si>
@@ -970,9 +930,6 @@
     <t>R3,R7,R8,R9</t>
   </si>
   <si>
-    <t>R1,R2,R10,R11</t>
-  </si>
-  <si>
     <t>390k resistor</t>
   </si>
   <si>
@@ -1009,40 +966,307 @@
     <t>C1,C8,C9,C18</t>
   </si>
   <si>
-    <t>BUTTON-GULLWING</t>
-  </si>
-  <si>
     <t>SW1,SW2</t>
   </si>
   <si>
     <t>SW3,SW4,SW5</t>
   </si>
   <si>
-    <t>TACTILE_SWITCH_SMD_6.2MM_TALL</t>
-  </si>
-  <si>
     <t>10uH Inductor</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>XTAL1</t>
-  </si>
-  <si>
     <t>32.768kHz Oscillator</t>
   </si>
   <si>
-    <t>2-SMD.NOLEAD.2.0MMTO1.2MM (Version 1 + Edits)</t>
-  </si>
-  <si>
-    <t>RED SMD LED</t>
-  </si>
-  <si>
     <t>LED2</t>
   </si>
   <si>
     <t>BLUE SMD LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>Red 622nm LED Indication - Discrete 2.2V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>Inolux</t>
+  </si>
+  <si>
+    <t>IN-S63ATR</t>
+  </si>
+  <si>
+    <t>1830-1065-1-ND</t>
+  </si>
+  <si>
+    <t>Blue 470nm LED Indication - Discrete 3V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>IN-S63AT5B</t>
+  </si>
+  <si>
+    <t>1830-1061-1-ND</t>
+  </si>
+  <si>
+    <t>0.96" OLED</t>
+  </si>
+  <si>
+    <t>OLED</t>
+  </si>
+  <si>
+    <t>Datasheet 128x64 OLED Module SPI 0.96"Graphic Displays,White on Black</t>
+  </si>
+  <si>
+    <t>Flexible Connector</t>
+  </si>
+  <si>
+    <t>EastRising</t>
+  </si>
+  <si>
+    <t>https://www.buydisplay.com/datasheet-128x64-oled-module-spi-0-96-inch-graphic-displays-white-on-black</t>
+  </si>
+  <si>
+    <t>BuyDisplay.com</t>
+  </si>
+  <si>
+    <t>R1,R2,R6,R10,R11</t>
+  </si>
+  <si>
+    <t>12pF capacitor</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>10µH Shielded Multilayer Inductor 250mA 1.05Ohm 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>MLZ1608M100WTD25</t>
+  </si>
+  <si>
+    <t>DEBUG1</t>
+  </si>
+  <si>
+    <t>Cortex Debug Connector - 10 pin</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 10 position 0.050" (1.27mm)</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>20021111-00010T4LF</t>
+  </si>
+  <si>
+    <t>609-3712-ND</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>Diode Schottky 30V 1.5A Surface Mount USC</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>CUS15S30,H3F</t>
+  </si>
+  <si>
+    <t>CUS15S30H3FCT-ND</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>PCF8523</t>
+  </si>
+  <si>
+    <t>XTAL1, XTAL2</t>
+  </si>
+  <si>
+    <t>Real Time Clock (RTC) IC Clock/Calendar I²C, 2-Wire Serial 8-SOIC (0.154", 3.90mm Width)</t>
+  </si>
+  <si>
+    <t>8-SO</t>
+  </si>
+  <si>
+    <t>NXP USA Inc.</t>
+  </si>
+  <si>
+    <t>PCF8523T/1,118</t>
+  </si>
+  <si>
+    <t>568-5306-1-ND</t>
+  </si>
+  <si>
+    <t>D1,D2,D3</t>
+  </si>
+  <si>
+    <t>LDO1</t>
+  </si>
+  <si>
+    <t>CHRG1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3V</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC 1 Output 300mA SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>576-4764-1-ND</t>
+  </si>
+  <si>
+    <t>MCP73831 T Li-Ion, Li-Pol Controller</t>
+  </si>
+  <si>
+    <t>Charger IC Lithium-Ion/Polymer SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OTCT-ND</t>
+  </si>
+  <si>
+    <t>Tiny Rectangular Switch</t>
+  </si>
+  <si>
+    <t>Tactile Switch SPST-NO Top Actuated Surface Mount</t>
+  </si>
+  <si>
+    <t>Gull Wing</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>PTS830GM140 SMTR LFS</t>
+  </si>
+  <si>
+    <t>CKN10587CT-ND</t>
+  </si>
+  <si>
+    <t>SWITCH.MOM (TACTILE_SWITCH_SMD_6.2MM_TALL)</t>
+  </si>
+  <si>
+    <t>Tactile Switch SPST-NO Top Actuated Surface Mount - TACT 4.5 X 4.5, 5.0 MM H, 1.0N,</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>PTS 647 SN50 SMTR2 LFS</t>
+  </si>
+  <si>
+    <t>PTS647SN50SMTR2LFSCT-ND</t>
+  </si>
+  <si>
+    <t>32.768kHz ±10ppm Crystal 12.5pF 90 kOhms 2-SMD, No Lead</t>
+  </si>
+  <si>
+    <t>2-SMD, No Lead</t>
+  </si>
+  <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>ECS-.327-12.5-12-C-TR</t>
+  </si>
+  <si>
+    <t>XC2288CT-ND</t>
+  </si>
+  <si>
+    <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>1 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K00</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K00CT-ND</t>
+  </si>
+  <si>
+    <t>390 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FG390K</t>
+  </si>
+  <si>
+    <t>RMCF0603FG390KCT-ND</t>
+  </si>
+  <si>
+    <t>10 µF ±10% 25V Ceramic Capacitor X5R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
+    <t>08053D106KAT4A</t>
+  </si>
+  <si>
+    <t>478-08053D106KAT4ATR-ND</t>
+  </si>
+  <si>
+    <t>0.1µF ±5% 16V Ceramic Capacitor X7R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R7BB104</t>
+  </si>
+  <si>
+    <t>311-1776-1-ND</t>
+  </si>
+  <si>
+    <t>12pF ±5% 50V Ceramic Capacitor C0G, NP0 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>Walsin Technology Corporation</t>
+  </si>
+  <si>
+    <t>0603N120J500CT</t>
+  </si>
+  <si>
+    <t>1292-1480-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1277,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1126,6 +1350,18 @@
     <font>
       <sz val="8"/>
       <color rgb="FF444444"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Segoe UI Historic"/>
       <family val="2"/>
     </font>
@@ -1295,7 +1531,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1324,6 +1560,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,10 +1572,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1757,15 +1994,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.34765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.94921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.84765625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.84765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.6484375" style="1" bestFit="1" customWidth="1"/>
@@ -1781,12 +2018,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="14.7" x14ac:dyDescent="0.65">
-      <c r="A1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
+      <c r="A1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1799,14 +2036,14 @@
       </c>
       <c r="M1" s="6">
         <f>SUM(M3:M77)</f>
-        <v>10.700000000000001</v>
+        <v>23.339999999999996</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" s="6">
         <f>SUM(O3:O77)</f>
-        <v>9.9516000000000009</v>
+        <v>19.678400000000003</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
@@ -1862,31 +2099,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" s="10">
         <v>9.9</v>
@@ -1902,7 +2139,7 @@
         <v>9.9</v>
       </c>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O7" si="1">L3*N3</f>
+        <f>L3*N3</f>
         <v>9.9</v>
       </c>
     </row>
@@ -1911,32 +2148,48 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
+      <c r="J4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="L4" s="11">
+        <v>2</v>
+      </c>
       <c r="M4" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="10"/>
+        <v>1.42</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="O4" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="O4:O27" si="1">L4*N4</f>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
@@ -1944,32 +2197,48 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="E5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="F5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
+      <c r="J5" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="L5" s="11">
+        <v>3</v>
+      </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="10"/>
+        <v>0.63</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.17</v>
+      </c>
       <c r="O5" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
@@ -1977,34 +2246,48 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="I6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
+      <c r="J6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="L6" s="11">
+        <v>1</v>
+      </c>
       <c r="M6" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="10"/>
+        <v>0.22</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0.22</v>
+      </c>
       <c r="O6" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
@@ -2015,10 +2298,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>12</v>
@@ -2030,30 +2313,30 @@
         <v>18</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="10">
         <v>0.1</v>
       </c>
       <c r="L7" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="N7" s="10">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O7" s="10">
         <f t="shared" si="1"/>
-        <v>2.7199999999999998E-2</v>
+        <v>3.3999999999999996E-2</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="12.3" x14ac:dyDescent="0.55000000000000004">
@@ -2064,7 +2347,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>20</v>
@@ -2090,33 +2373,35 @@
       <c r="K8" s="10">
         <v>0.1</v>
       </c>
-      <c r="L8" s="11"/>
+      <c r="L8" s="11">
+        <v>4</v>
+      </c>
       <c r="M8" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N8" s="10">
-        <v>1.8499999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="O8" s="10">
-        <f>L8*N8</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
+      <c r="B9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -2125,14 +2410,14 @@
       <c r="G9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>40</v>
+      <c r="H9" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" s="10">
         <v>0.1</v>
@@ -2148,7 +2433,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
       <c r="O9" s="10">
-        <f>L9*N9</f>
+        <f t="shared" si="1"/>
         <v>2.4400000000000002E-2</v>
       </c>
     </row>
@@ -2157,12 +2442,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>12</v>
       </c>
@@ -2172,21 +2459,31 @@
       <c r="G10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>139</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
+      <c r="J10" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="11">
+        <v>2</v>
+      </c>
       <c r="M10" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="10"/>
+        <v>0.2</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0.01</v>
+      </c>
       <c r="O10" s="10">
-        <f t="shared" ref="O10" si="3">L10*N10</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
@@ -2194,12 +2491,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>141</v>
+      </c>
       <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
@@ -2209,76 +2508,98 @@
       <c r="G11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="I11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
+      <c r="J11" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
       <c r="M11" s="10">
-        <f t="shared" ref="M11:M15" si="4">K11*L11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="10"/>
+        <f t="shared" ref="M11:M14" si="3">K11*L11</f>
+        <v>0.16</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0.05</v>
+      </c>
       <c r="O11" s="10">
-        <f t="shared" ref="O11" si="5">L11*N11</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="I12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
+      <c r="J12" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
       <c r="M12" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="10"/>
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0.2</v>
+      </c>
       <c r="O12" s="10">
-        <f>L12*N12</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>17</v>
@@ -2288,25 +2609,29 @@
         <v>9</v>
       </c>
       <c r="J13" s="9"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
       <c r="M13" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10">
-        <f>L13*N13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9" t="s">
@@ -2323,27 +2648,33 @@
         <v>9</v>
       </c>
       <c r="J14" s="9"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="2">
+        <v>2</v>
+      </c>
       <c r="M14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10">
-        <f>L14*N14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
@@ -2351,34 +2682,48 @@
         <v>16</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="9"/>
+        <v>149</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="I15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
       <c r="M15" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="10"/>
+        <f t="shared" ref="M15:M18" si="4">K15*L15</f>
+        <v>0.1</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0.03</v>
+      </c>
       <c r="O15" s="10">
-        <f>L15*N15</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>152</v>
+      </c>
       <c r="E16" s="9" t="s">
         <v>12</v>
       </c>
@@ -2386,201 +2731,557 @@
         <v>16</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="I16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2</v>
+      </c>
       <c r="M16" s="10">
-        <f t="shared" ref="M16:M17" si="6">K16*L16</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="10"/>
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="N16" s="10">
+        <v>0.01</v>
+      </c>
       <c r="O16" s="10">
-        <f>L16*N16</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="I17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2</v>
+      </c>
       <c r="M17" s="10">
+        <f t="shared" si="4"/>
+        <v>1.66</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="O17" s="10">
+        <f t="shared" si="1"/>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="O18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" ref="M19:M22" si="5">K19*L19</f>
+        <v>0.33</v>
+      </c>
+      <c r="N19" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="13.5" x14ac:dyDescent="0.6">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="10">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="5"/>
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="N20" s="10">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0.79</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="5"/>
+        <v>0.79</v>
+      </c>
+      <c r="N21" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="O21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="L22" s="2">
+        <v>3</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="5"/>
+        <v>0.78</v>
+      </c>
+      <c r="N22" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="O22" s="10">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K23" s="10">
+        <v>1.26</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="10">
+        <f t="shared" ref="M23:M27" si="6">K23*L23</f>
+        <v>1.26</v>
+      </c>
+      <c r="N23" s="10">
+        <v>1.26</v>
+      </c>
+      <c r="O23" s="10">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="10">
+        <f t="shared" si="6"/>
+        <v>0.11</v>
+      </c>
+      <c r="N24" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="O24" s="10">
+        <f t="shared" si="1"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="M25" s="10">
+        <f t="shared" si="6"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N25" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O25" s="10">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10">
-        <f>L17*N17</f>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="9"/>
-      <c r="M18" s="10">
-        <f t="shared" ref="M18:M22" si="7">K18*L18</f>
+    <row r="27" spans="1:15" ht="12.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="M27" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10">
-        <f>L18*N18</f>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A19" s="8">
-        <v>17</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="M19" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10">
-        <f t="shared" ref="O19:O22" si="8">L19*N19</f>
-        <v>0</v>
-      </c>
+    <row r="28" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="K28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
     </row>
-    <row r="20" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A20" s="8">
-        <v>18</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="9"/>
-      <c r="M20" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="K29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
     </row>
-    <row r="21" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A21" s="8">
-        <v>19</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="M21" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A22" s="8">
-        <v>20</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="M22" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
+    <row r="30" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="K30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>